<commit_message>
Added new hazard HA-004 with relevant description an safety goal.
</commit_message>
<xml_diff>
--- a/02_HazardAnalysisAndRiskAssessment.xlsx
+++ b/02_HazardAnalysisAndRiskAssessment.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="285">
   <si>
     <t>Hazard &amp; Risk Analysis Definitions</t>
   </si>
@@ -310,9 +310,6 @@
     <t>road type</t>
   </si>
   <si>
-    <t>EV00 - Collition with other vehicle.</t>
-  </si>
-  <si>
     <t>High haptic feedback can affect driver's ability to steer as intented. The driver loose control and could collide with another vehicle or side of the road.</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
     <t>S3 - Life-threatening or fatal injuries</t>
   </si>
   <si>
-    <t>Collitions at high speed could cause fatal injuries.</t>
-  </si>
-  <si>
     <t>Country Road</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
     <t>IU02 - Incorrectly used</t>
   </si>
   <si>
-    <t>Normal driving on a country road during normal conditions with high speed and incorrectly used systam.</t>
-  </si>
-  <si>
     <t>Lane Keeping Assistance (LKA) function shall apply the steering torque when active in order to stay in ego lane</t>
   </si>
   <si>
@@ -409,9 +400,6 @@
     <t>The conviation beween driving at a country road and misusing system should not happen oftern. Less than 1% of the time operating the vehicle.</t>
   </si>
   <si>
-    <t>When the driver loose focus on driving, it is difficult to re-focus in the case of inmminent collition.</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -430,9 +418,6 @@
     <t>The camera sensor stop working and the Lane Departure Warning function continue to be activated.</t>
   </si>
   <si>
-    <t>The Lane Departure Warning continue to be activated and start executing random torque to the steering wheel making the driver to loose control with potential collition with other vehicle.</t>
-  </si>
-  <si>
     <t>The Lane Departure Warning start acting randomly when the camera sensor is not working.</t>
   </si>
   <si>
@@ -454,9 +439,6 @@
     <t>OS01 - City Road</t>
   </si>
   <si>
-    <t>Normal driving on a country road during normal conditions with high speed and correctly used system.</t>
-  </si>
-  <si>
     <t>SD03 - Low speed</t>
   </si>
   <si>
@@ -466,21 +448,12 @@
     <t>DV01 - Function not activated</t>
   </si>
   <si>
-    <t>The Lane Keeping Assistance continue to be activated starting executing random torque to the vehicle making the driver to loose control with potential collition with other vehicle.</t>
-  </si>
-  <si>
     <t>EV04 - Front collision with obstacle</t>
   </si>
   <si>
-    <t>The Lane Keeping Assistance start acting randomly when the camera sensor is not working.</t>
-  </si>
-  <si>
     <t>High speed</t>
   </si>
   <si>
-    <t>The Lane Keeping Assistance function shall be deactivated when the camera sensor stop working.</t>
-  </si>
-  <si>
     <t>Normal acceleration</t>
   </si>
   <si>
@@ -892,7 +865,57 @@
     <t>D</t>
   </si>
   <si>
-    <t>Lane Keeping Assistance prevents the driver from leaving the lane when there's an obstacle ahead.</t>
+    <t>EV00 - collision with other vehicle.</t>
+  </si>
+  <si>
+    <t>collisions at high speed could cause fatal injuries.</t>
+  </si>
+  <si>
+    <t>When the driver loose focus on driving, it is difficult to re-focus in the case of inmminent collision.</t>
+  </si>
+  <si>
+    <t>The Lane Departure Warning continue to be activated and start executing random torque to the steering wheel making the driver to loose control with potential collision with other vehicle.</t>
+  </si>
+  <si>
+    <t>Normal driving on a country road during normal conditions with high speed and incorrectly used system.</t>
+  </si>
+  <si>
+    <t>EN05-  Cross-wind (lateral force)</t>
+  </si>
+  <si>
+    <t>Normal Driving on a highway during strong
+winds with high speed and correctly used
+system</t>
+  </si>
+  <si>
+    <t>DV05 - Actor effect is
+too less</t>
+  </si>
+  <si>
+    <t>If the direction of strong wind is opposite to the direction of torque applied to keep the vehicle in lane, the amount of torque applied maybe too small to keep the vehicle in lane</t>
+  </si>
+  <si>
+    <t>If the amount of torque applied is not sufficient to keep the vehicle in lane, the vehicle might be in the lane boundary and could collide with other vehicles.</t>
+  </si>
+  <si>
+    <t>Amount of torque applied is smaller than what is required to keep the vehicle in lane</t>
+  </si>
+  <si>
+    <t>Highway Driving on windy roads.</t>
+  </si>
+  <si>
+    <t>Driver travelling at high
+speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver can control the vehicle and steer it into the
+right lane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2 - Normally controllable. </t>
+  </si>
+  <si>
+    <t>The lane keeping assistance function shall apply a higher torque when the prevailing winds is in the direction opposite to the direction of application of torque</t>
   </si>
 </sst>
 </file>
@@ -1682,7 +1705,7 @@
   <dimension ref="A1:AB991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1752,7 +1775,7 @@
       <c r="AA1" s="9"/>
       <c r="AB1" s="9"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -1824,7 +1847,7 @@
       <c r="AA2" s="13"/>
       <c r="AB2" s="13"/>
     </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" ht="90" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
@@ -1857,37 +1880,37 @@
         <v>81</v>
       </c>
       <c r="L3" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="M3" s="16" t="s">
         <v>84</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="N3" s="16" t="s">
         <v>81</v>
       </c>
       <c r="O3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="16" t="s">
-        <v>88</v>
-      </c>
       <c r="R3" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="S3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="T3" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="U3" s="25" t="s">
-        <v>93</v>
-      </c>
       <c r="V3" s="26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W3" s="27"/>
       <c r="X3" s="27"/>
@@ -1896,70 +1919,70 @@
       <c r="AA3" s="28"/>
       <c r="AB3" s="28"/>
     </row>
-    <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" ht="90" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="K4" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="L4" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="N4" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="O4" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" s="16" t="s">
+      <c r="P4" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="Q4" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="U4" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="V4" s="26" t="s">
         <v>115</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="S4" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="T4" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="U4" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="V4" s="26" t="s">
-        <v>119</v>
       </c>
       <c r="W4" s="27"/>
       <c r="X4" s="27"/>
@@ -1968,9 +1991,9 @@
       <c r="AA4" s="28"/>
       <c r="AB4" s="28"/>
     </row>
-    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="90" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>36</v>
@@ -1979,7 +2002,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>48</v>
@@ -1989,49 +2012,49 @@
         <v>77</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>79</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>84</v>
+        <v>269</v>
       </c>
       <c r="M5" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="U5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="V5" s="26" t="s">
         <v>124</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="U5" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="V5" s="26" t="s">
-        <v>129</v>
       </c>
       <c r="W5" s="27"/>
       <c r="X5" s="27"/>
@@ -2040,20 +2063,20 @@
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
     </row>
-    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="14" t="s">
-        <v>130</v>
+    <row r="6" spans="1:28" ht="90" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="25" t="s">
+        <v>125</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="C6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="21"/>
@@ -2061,49 +2084,49 @@
         <v>77</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>132</v>
+        <v>275</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>122</v>
+        <v>276</v>
       </c>
       <c r="K6" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="M6" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="L6" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>136</v>
-      </c>
       <c r="N6" s="16" t="s">
-        <v>138</v>
+        <v>279</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P6" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q6" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>88</v>
-      </c>
       <c r="R6" s="16" t="s">
-        <v>89</v>
+        <v>281</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>91</v>
+        <v>283</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>126</v>
+        <v>282</v>
       </c>
       <c r="U6" s="25" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="V6" s="26" t="s">
-        <v>140</v>
+        <v>284</v>
       </c>
       <c r="W6" s="27"/>
       <c r="X6" s="27"/>
@@ -3114,7 +3137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0"/>
+    <sheetView topLeftCell="J1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3271,7 +3294,7 @@
       </c>
       <c r="W4" s="55"/>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
@@ -3514,7 +3537,7 @@
     <row r="10" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -3580,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D12" s="53"/>
       <c r="E12" s="53"/>
@@ -3615,7 +3638,7 @@
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
     </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" ht="49" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
         <v>3</v>
@@ -3695,13 +3718,13 @@
         <v>36</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>59</v>
@@ -3710,19 +3733,19 @@
         <v>77</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>62</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L14" s="19" t="s">
         <v>64</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="N14" s="19" t="s">
         <v>66</v>
@@ -3752,7 +3775,7 @@
         <v>74</v>
       </c>
       <c r="W14" s="22" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="X14" s="24"/>
       <c r="Y14" s="24"/>
@@ -3763,40 +3786,40 @@
     </row>
     <row r="15" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>77</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>62</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L15" s="19" t="s">
         <v>64</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="N15" s="19" t="s">
         <v>66</v>
@@ -3805,10 +3828,10 @@
         <v>67</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="R15" s="19" t="s">
         <v>70</v>
@@ -3817,16 +3840,16 @@
         <v>71</v>
       </c>
       <c r="T15" s="19" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="U15" s="19" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="V15" s="19" t="s">
         <v>74</v>
       </c>
       <c r="W15" s="22" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="X15" s="24"/>
       <c r="Y15" s="24"/>
@@ -3837,70 +3860,70 @@
     </row>
     <row r="16" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>77</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>62</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>64</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>67</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="R16" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S16" s="19" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="T16" s="19" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="U16" s="19" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="V16" s="19" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="W16" s="22" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="X16" s="24"/>
       <c r="Y16" s="24"/>
@@ -3911,43 +3934,43 @@
     </row>
     <row r="17" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>77</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>62</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L17" s="19" t="s">
         <v>64</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="O17" s="19" t="s">
         <v>67</v>
@@ -3956,25 +3979,25 @@
         <v>68</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="R17" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S17" s="19" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="T17" s="19" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="U17" s="19" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="V17" s="19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="W17" s="22" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="X17" s="24"/>
       <c r="Y17" s="24"/>
@@ -3985,70 +4008,70 @@
     </row>
     <row r="18" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="19" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>77</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>62</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L18" s="19" t="s">
         <v>64</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>67</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="R18" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S18" s="19" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="T18" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="U18" s="19" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="V18" s="19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="W18" s="22" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="X18" s="24"/>
       <c r="Y18" s="24"/>
@@ -5142,7 +5165,7 @@
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5150,7 +5173,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:B55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5611,7 +5636,7 @@
         <v>OS03</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>83</v>
@@ -5637,7 +5662,7 @@
         <v>OS04</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>83</v>
@@ -5663,7 +5688,7 @@
         <v>OS05</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>83</v>
@@ -5689,7 +5714,7 @@
         <v>OS06</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>83</v>
@@ -5715,10 +5740,10 @@
         <v>OS07</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="D24" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5741,10 +5766,10 @@
         <v>OS08</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D25" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5767,10 +5792,10 @@
         <v>OS09</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D26" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5793,10 +5818,10 @@
         <v>OS10</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D27" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5919,10 +5944,10 @@
         <v>SD01</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D33" s="15" t="str">
         <f t="shared" ref="D33:D39" si="5">$A33 &amp; " - " &amp; $B33</f>
@@ -5945,10 +5970,10 @@
         <v>SD02</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D34" s="15" t="str">
         <f t="shared" si="5"/>
@@ -5971,10 +5996,10 @@
         <v>SD03</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D35" s="15" t="str">
         <f t="shared" si="5"/>
@@ -5997,10 +6022,10 @@
         <v>SD04</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D36" s="15" t="str">
         <f t="shared" si="5"/>
@@ -6023,10 +6048,10 @@
         <v>SD05</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D37" s="15" t="str">
         <f t="shared" si="5"/>
@@ -6049,10 +6074,10 @@
         <v>SD06</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D38" s="15" t="str">
         <f t="shared" si="5"/>
@@ -6129,7 +6154,7 @@
     </row>
     <row r="42" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -6175,10 +6200,10 @@
         <v>IU01</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D44" s="15" t="str">
         <f t="shared" ref="D44:D46" si="7">$A44 &amp; " - " &amp; $B44</f>
@@ -6201,10 +6226,10 @@
         <v>IU02</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D45" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6327,10 +6352,10 @@
         <v>EN01</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D51" s="15" t="str">
         <f t="shared" ref="D51:D59" si="9">$A51 &amp; " - " &amp; $B51</f>
@@ -6353,10 +6378,10 @@
         <v>EN02</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D52" s="15" t="str">
         <f t="shared" si="9"/>
@@ -6379,10 +6404,10 @@
         <v>EN03</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D53" s="15" t="str">
         <f t="shared" si="9"/>
@@ -6405,10 +6430,10 @@
         <v>EN04</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D54" s="15" t="str">
         <f t="shared" si="9"/>
@@ -6431,10 +6456,10 @@
         <v>EN05</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D55" s="15" t="str">
         <f t="shared" si="9"/>
@@ -6457,10 +6482,10 @@
         <v>EN06</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D56" s="15" t="str">
         <f t="shared" si="9"/>
@@ -6483,10 +6508,10 @@
         <v>EN07</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D57" s="15" t="str">
         <f t="shared" si="9"/>
@@ -6509,10 +6534,10 @@
         <v>EN08</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D58" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7812,7 +7837,7 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7820,7 +7845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A12" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7870,7 +7895,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>7</v>
@@ -7898,7 +7923,7 @@
         <v>63</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D4" s="15" t="str">
         <f t="shared" ref="D4:D23" si="1">$A4 &amp; " - " &amp; $B4</f>
@@ -7921,10 +7946,10 @@
         <v>DV02</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D5" s="15" t="str">
         <f t="shared" si="1"/>
@@ -7947,10 +7972,10 @@
         <v>DV03</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D6" s="15" t="str">
         <f t="shared" si="1"/>
@@ -7973,10 +7998,10 @@
         <v>DV04</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D7" s="15" t="str">
         <f t="shared" si="1"/>
@@ -7999,10 +8024,10 @@
         <v>DV05</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D8" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8025,10 +8050,10 @@
         <v>DV06</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D9" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8051,10 +8076,10 @@
         <v>DV07</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D10" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8077,10 +8102,10 @@
         <v>DV08</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D11" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8103,10 +8128,10 @@
         <v>DV09</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D12" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8129,10 +8154,10 @@
         <v>DV10</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D13" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8155,10 +8180,10 @@
         <v>DV11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D14" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8181,10 +8206,10 @@
         <v>DV12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D15" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8207,10 +8232,10 @@
         <v>DV13</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D16" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8233,10 +8258,10 @@
         <v>DV14</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D17" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8259,10 +8284,10 @@
         <v>DV15</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="D18" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8285,10 +8310,10 @@
         <v>DV16</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D19" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8311,10 +8336,10 @@
         <v>DV17</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D20" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8337,10 +8362,10 @@
         <v>DV18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D21" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8363,10 +8388,10 @@
         <v>DV19</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D22" s="15" t="str">
         <f t="shared" si="1"/>
@@ -8443,7 +8468,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="39" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
@@ -8464,7 +8489,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>7</v>
@@ -8489,7 +8514,7 @@
         <v>EV-07</v>
       </c>
       <c r="B28" s="44" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C28" s="45"/>
       <c r="D28" s="46" t="str">
@@ -8513,7 +8538,7 @@
         <v>EV-06</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C29" s="45"/>
       <c r="D29" s="46" t="str">
@@ -8537,7 +8562,7 @@
         <v>EV-05</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C30" s="45"/>
       <c r="D30" s="46" t="str">
@@ -8585,7 +8610,7 @@
         <v>EV-03</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C32" s="45"/>
       <c r="D32" s="46" t="str">
@@ -8609,7 +8634,7 @@
         <v>EV-02</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C33" s="45"/>
       <c r="D33" s="46" t="str">
@@ -8633,7 +8658,7 @@
         <v>EV-01</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C34" s="45"/>
       <c r="D34" s="46" t="str">
@@ -8657,7 +8682,7 @@
         <v>EV00</v>
       </c>
       <c r="B35" s="44" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C35" s="45"/>
       <c r="D35" s="46" t="str">
@@ -8681,7 +8706,7 @@
         <v>EV01</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C36" s="45"/>
       <c r="D36" s="46" t="str">
@@ -8705,7 +8730,7 @@
         <v>EV02</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C37" s="45"/>
       <c r="D37" s="46" t="str">
@@ -8729,7 +8754,7 @@
         <v>EV03</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C38" s="45"/>
       <c r="D38" s="46" t="str">
@@ -8753,7 +8778,7 @@
         <v>EV04</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C39" s="45"/>
       <c r="D39" s="46" t="str">
@@ -8777,7 +8802,7 @@
         <v>EV05</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C40" s="45"/>
       <c r="D40" s="46" t="str">
@@ -11281,7 +11306,7 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -11289,7 +11314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11302,7 +11329,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -11324,13 +11351,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>8</v>
@@ -11348,10 +11375,10 @@
     </row>
     <row r="3" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -11372,16 +11399,16 @@
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E4" s="15" t="str">
         <f t="shared" si="0"/>
@@ -11400,16 +11427,16 @@
     </row>
     <row r="5" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="31" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E5" s="15" t="str">
         <f t="shared" si="0"/>
@@ -11428,16 +11455,16 @@
     </row>
     <row r="6" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E6" s="15" t="str">
         <f t="shared" si="0"/>
@@ -11456,16 +11483,16 @@
     </row>
     <row r="7" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E7" s="15" t="str">
         <f t="shared" si="0"/>
@@ -11518,7 +11545,7 @@
     </row>
     <row r="10" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -11540,13 +11567,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>8</v>
@@ -11564,16 +11591,16 @@
     </row>
     <row r="12" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="31" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E12" s="15" t="str">
         <f t="shared" ref="E12:E15" si="1">$A12 &amp; " - " &amp; $B12</f>
@@ -11592,16 +11619,16 @@
     </row>
     <row r="13" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="31" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="E13" s="15" t="str">
         <f t="shared" si="1"/>
@@ -11620,16 +11647,16 @@
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="31" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E14" s="15" t="str">
         <f t="shared" si="1"/>
@@ -11648,16 +11675,16 @@
     </row>
     <row r="15" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="31" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E15" s="15" t="str">
         <f t="shared" si="1"/>
@@ -11710,7 +11737,7 @@
     </row>
     <row r="18" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -11732,7 +11759,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>7</v>
@@ -11754,13 +11781,13 @@
     </row>
     <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="15" t="str">
@@ -11780,13 +11807,13 @@
     </row>
     <row r="21" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="15" t="str">
@@ -11806,13 +11833,13 @@
     </row>
     <row r="22" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="31" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="15" t="str">
@@ -11832,13 +11859,13 @@
     </row>
     <row r="23" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="31" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="15" t="str">
@@ -12852,7 +12879,7 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -12870,13 +12897,13 @@
     <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="59" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E2" s="63"/>
       <c r="F2" s="63"/>
@@ -12886,24 +12913,24 @@
       <c r="B3" s="58"/>
       <c r="C3" s="61"/>
       <c r="D3" s="45" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="56" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>74</v>
@@ -12921,7 +12948,7 @@
     <row r="5" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="57"/>
       <c r="C5" s="47" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D5" s="47" t="s">
         <v>74</v>
@@ -12939,7 +12966,7 @@
     <row r="6" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="57"/>
       <c r="C6" s="47" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D6" s="47" t="s">
         <v>74</v>
@@ -12951,13 +12978,13 @@
         <v>74</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="58"/>
       <c r="C7" s="47" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D7" s="47" t="s">
         <v>74</v>
@@ -12966,18 +12993,18 @@
         <v>74</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G7" s="47" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="56" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D8" s="47" t="s">
         <v>74</v>
@@ -12995,7 +13022,7 @@
     <row r="9" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="57"/>
       <c r="C9" s="47" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D9" s="47" t="s">
         <v>74</v>
@@ -13007,13 +13034,13 @@
         <v>74</v>
       </c>
       <c r="G9" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="57"/>
       <c r="C10" s="47" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D10" s="47" t="s">
         <v>74</v>
@@ -13022,36 +13049,36 @@
         <v>74</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G10" s="47" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="58"/>
       <c r="C11" s="47" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>74</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F11" s="47" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="56" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>74</v>
@@ -13063,13 +13090,13 @@
         <v>74</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="57"/>
       <c r="C13" s="47" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D13" s="47" t="s">
         <v>74</v>
@@ -13078,46 +13105,46 @@
         <v>74</v>
       </c>
       <c r="F13" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G13" s="47" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="57"/>
       <c r="C14" s="47" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D14" s="47" t="s">
         <v>74</v>
       </c>
       <c r="E14" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F14" s="47" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G14" s="47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="58"/>
       <c r="C15" s="47" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D15" s="47" t="s">
         <v>74</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F15" s="47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14116,6 +14143,6 @@
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>